<commit_message>
Added all instructions to main loop (some need to be done)
</commit_message>
<xml_diff>
--- a/ref/Insn-ASCII conversion.xlsx
+++ b/ref/Insn-ASCII conversion.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\adityasrinivasan\fpga-logo\ref\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adityasrinivasan/Documents/GitHub/fpga-logo/ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10350"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>FWD</t>
   </si>
@@ -38,12 +44,6 @@
     <t>RRT</t>
   </si>
   <si>
-    <t>UND</t>
-  </si>
-  <si>
-    <t>RDO</t>
-  </si>
-  <si>
     <t>CLC</t>
   </si>
   <si>
@@ -86,12 +86,6 @@
     <t>010101010100111001000100</t>
   </si>
   <si>
-    <t>52444f</t>
-  </si>
-  <si>
-    <t>010100100100010001001111</t>
-  </si>
-  <si>
     <t>434c43</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>5590596</t>
   </si>
   <si>
-    <t>5391439</t>
-  </si>
-  <si>
     <t>CTI</t>
   </si>
   <si>
@@ -144,12 +135,45 @@
   </si>
   <si>
     <t>remainder</t>
+  </si>
+  <si>
+    <t>524544</t>
+  </si>
+  <si>
+    <t>5391684</t>
+  </si>
+  <si>
+    <t>010100100100010101000100</t>
+  </si>
+  <si>
+    <t>PNUP</t>
+  </si>
+  <si>
+    <t>PNDN</t>
+  </si>
+  <si>
+    <t>50 4e 55</t>
+  </si>
+  <si>
+    <t>01010000 01001110 01010101</t>
+  </si>
+  <si>
+    <t>50 4e 44</t>
+  </si>
+  <si>
+    <t>01010000 01001110 01000100</t>
+  </si>
+  <si>
+    <t>UNDO</t>
+  </si>
+  <si>
+    <t>REDO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -462,38 +486,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:I14"/>
+  <dimension ref="B4:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -501,10 +525,10 @@
         <v>465744</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <f>SQRT(D5)</f>
@@ -523,18 +547,18 @@
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <f t="shared" ref="F6:F11" si="0">SQRT(D6)</f>
@@ -553,18 +577,18 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -583,18 +607,18 @@
         <v>2116</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -613,18 +637,18 @@
         <v>-1301</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
@@ -643,22 +667,22 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>2321.9472431560544</v>
+        <v>2322</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
@@ -670,21 +694,21 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" si="3"/>
-        <v>-245</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
@@ -703,37 +727,145 @@
         <v>-1712</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f>SQRT(D12)</f>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f>ROUND(F12, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f>G12*G12</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f>D12-H12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:F14" si="4">SQRT(D13)</f>
+        <v>2100.1035688746401</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13:G14" si="5">ROUND(F13, 0)</f>
+        <v>2100</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13:H14" si="6">G13*G13</f>
+        <v>4410000</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" ref="I13:I14" si="7">D13-H13</f>
+        <v>435</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>2322.6097390650889</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>2323</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="6"/>
+        <v>5396329</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="7"/>
+        <v>-1813</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15">
+        <v>5262933</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F15" si="8">SQRT(D15)</f>
+        <v>2294.1083235104657</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ref="G15" si="9">ROUND(F15, 0)</f>
+        <v>2294</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15" si="10">G15*G15</f>
+        <v>5262436</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" ref="I15" si="11">D15-H15</f>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16">
+        <v>5262916</v>
+      </c>
+      <c r="E16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16" si="12">SQRT(D16)</f>
+        <v>2294.1046183642106</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16" si="13">ROUND(F16, 0)</f>
+        <v>2294</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ref="H16" si="14">G16*G16</f>
+        <v>5262436</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" ref="I16" si="15">D16-H16</f>
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>